<commit_message>
Add question number to index.html
</commit_message>
<xml_diff>
--- a/server/survey_question_to_db/question_list.xlsx
+++ b/server/survey_question_to_db/question_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\project1\server\survey_question_to_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286FCE4A-B703-4C0F-BBC7-071D8A7F509B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A7DCD0-5289-4553-BF22-8FEF445FC6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{7CB90CA9-326C-44AC-B80A-E2BBE9E01591}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7CB90CA9-326C-44AC-B80A-E2BBE9E01591}"/>
   </bookViews>
   <sheets>
     <sheet name="자체제작" sheetId="3" r:id="rId1"/>
@@ -369,11 +369,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>평소에 사용하는 스킨케어 제품을 사용했을때, 
-가렵거나 화끈거린 경우가 있나요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스킨케어 제품을 사용하지 않아요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -604,6 +599,11 @@
   </si>
   <si>
     <t>최근 5년간 1시간 이상 실외에서 피부를 햇빛에 노출시킨 적이 있나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평소 스킨케어 제품을 사용했을때, 
+가렵거나 화끈거린 경우가 있나요?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -825,21 +825,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -851,10 +842,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1194,25 +1194,25 @@
   <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78:B81"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="49.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.25" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>19</v>
@@ -1245,7 +1245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="7" t="s">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="7" t="s">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
@@ -1302,24 +1302,24 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>94</v>
+      <c r="B6" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
-      <c r="B7" s="12"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1328,9 +1328,9 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1339,9 +1339,9 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1350,24 +1350,24 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
@@ -1376,17 +1376,17 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="12"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>4</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="7" t="s">
@@ -1424,7 +1424,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="7" t="s">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="5" t="s">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>5</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="4" t="s">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="4" t="s">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
@@ -1494,51 +1494,51 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>6</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G22" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>7</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="7" t="s">
@@ -1562,7 +1562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="7" t="s">
@@ -1575,7 +1575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="5" t="s">
@@ -1588,56 +1588,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>8</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="G30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A31" s="10"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="7" t="s">
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A32" s="10"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A33" s="10"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>9</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>40</v>
+      <c r="B34" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>37</v>
@@ -1646,9 +1646,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
-      <c r="B35" s="12"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="7" t="s">
         <v>38</v>
       </c>
@@ -1656,9 +1656,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="12"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="7" t="s">
         <v>39</v>
       </c>
@@ -1666,22 +1666,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
-      <c r="B37" s="13"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>10</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>42</v>
+      <c r="B38" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>37</v>
@@ -1690,9 +1690,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
-      <c r="B39" s="15"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="7" t="s">
         <v>38</v>
       </c>
@@ -1700,9 +1700,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
-      <c r="B40" s="15"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="7" t="s">
         <v>39</v>
       </c>
@@ -1710,25 +1710,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
-      <c r="B41" s="16"/>
+      <c r="B41" s="21"/>
       <c r="C41" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>11</v>
       </c>
-      <c r="B42" s="17" t="s">
-        <v>97</v>
+      <c r="B42" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I42" s="1">
         <v>4</v>
@@ -1736,11 +1736,11 @@
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
-      <c r="B43" s="18"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I43" s="1">
         <v>2</v>
@@ -1748,11 +1748,11 @@
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="18"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H44" s="1">
         <v>2</v>
@@ -1760,11 +1760,11 @@
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
-      <c r="B45" s="19"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H45" s="1">
         <v>4</v>
@@ -1772,56 +1772,56 @@
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>12</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I46" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I47" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H48" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H49" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
         <v>13</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>10</v>
@@ -1830,14 +1830,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="7" t="s">
@@ -1847,7 +1847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53" s="5" t="s">
@@ -1857,30 +1857,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="10">
         <v>14</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="H54" s="1">
+        <v>4</v>
+      </c>
+      <c r="J54" s="8">
+        <v>4</v>
+      </c>
+      <c r="K54" s="8"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="10"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="1">
-        <v>4</v>
-      </c>
-      <c r="J54" s="8">
-        <v>4</v>
-      </c>
-      <c r="K54" s="8"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A55" s="10"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="H55" s="1">
         <v>2</v>
       </c>
@@ -1889,11 +1889,11 @@
       </c>
       <c r="K55" s="8"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
-      <c r="B56" s="12"/>
+      <c r="B56" s="18"/>
       <c r="C56" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I56" s="1">
         <v>2</v>
@@ -1903,11 +1903,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
-      <c r="B57" s="13"/>
+      <c r="B57" s="19"/>
       <c r="C57" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I57" s="1">
         <v>4</v>
@@ -1917,15 +1917,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="10">
         <v>15</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I58" s="1">
         <v>4</v>
@@ -1935,11 +1935,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I59" s="1">
         <v>2</v>
@@ -1949,11 +1949,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H60" s="1">
         <v>2</v>
@@ -1963,11 +1963,11 @@
       </c>
       <c r="K60" s="8"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H61" s="1">
         <v>4</v>
@@ -1977,236 +1977,236 @@
       </c>
       <c r="K61" s="8"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="10">
         <v>16</v>
       </c>
       <c r="B62" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="K62" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K63" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J64" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J65" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="10">
         <v>17</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>88</v>
+      <c r="B66" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="C66" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K66" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="10"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K66" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A67" s="10"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="7" t="s">
+      <c r="K67" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="K67" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A68" s="10"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="7" t="s">
+      <c r="J68" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="10"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J68" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A69" s="10"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="J69" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="10">
         <v>18</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K70" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K71" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K70" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A71" s="10"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K71" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A72" s="10"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="7" t="s">
+      <c r="J72" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="J72" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A73" s="10"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="J73" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="10">
         <v>19</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="G74" s="8">
+        <v>4</v>
+      </c>
+      <c r="K74" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G74" s="8">
-        <v>4</v>
-      </c>
-      <c r="K74" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A75" s="10"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="7" t="s">
+      <c r="K75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="10"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K75" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A76" s="10"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="7" t="s">
+      <c r="F76" s="8">
+        <v>4</v>
+      </c>
+      <c r="J76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F76" s="8">
-        <v>4</v>
-      </c>
-      <c r="J76" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A77" s="10"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="J77" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="10">
         <v>20</v>
       </c>
-      <c r="B78" s="14" t="s">
-        <v>98</v>
+      <c r="B78" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C78" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I78" s="1">
+        <v>4</v>
+      </c>
+      <c r="K78" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I79" s="1">
+        <v>2</v>
+      </c>
+      <c r="K79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I78" s="1">
-        <v>4</v>
-      </c>
-      <c r="K78" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A79" s="10"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I79" s="1">
-        <v>2</v>
-      </c>
-      <c r="K79" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A80" s="10"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="7" t="s">
+      <c r="H80" s="1">
+        <v>2</v>
+      </c>
+      <c r="J80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="10"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="H80" s="1">
-        <v>2</v>
-      </c>
-      <c r="J80" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A81" s="10"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="H81" s="1">
         <v>4</v>
@@ -2217,6 +2217,31 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B50:B53"/>
     <mergeCell ref="A78:A81"/>
     <mergeCell ref="B78:B81"/>
     <mergeCell ref="B42:B45"/>
@@ -2232,31 +2257,6 @@
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A62:A65"/>
     <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>